<commit_message>
Tweaked the datasets to use same chord naming conventions
</commit_message>
<xml_diff>
--- a/Datasets/ChordLblStandard.xlsx
+++ b/Datasets/ChordLblStandard.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\CodingProjects\ChordRecognition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\CodingProjects\ChordRecognition\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
   <si>
     <t>maj</t>
   </si>
@@ -122,7 +122,67 @@
     <t>Group 3</t>
   </si>
   <si>
-    <t>Group 4</t>
+    <t>C-Eb-Gb</t>
+  </si>
+  <si>
+    <t>dim</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>d7</t>
+  </si>
+  <si>
+    <t>M7</t>
+  </si>
+  <si>
+    <t>m7</t>
+  </si>
+  <si>
+    <t>M4</t>
+  </si>
+  <si>
+    <t>m6</t>
+  </si>
+  <si>
+    <t>M6</t>
+  </si>
+  <si>
+    <t>OriginalBREVELabels</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>(deleted-d6)</t>
+  </si>
+  <si>
+    <t>hd7</t>
+  </si>
+  <si>
+    <t>KPLabels(29)</t>
+  </si>
+  <si>
+    <t>Style2</t>
+  </si>
+  <si>
+    <t>Style1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>mM7</t>
   </si>
 </sst>
 </file>
@@ -441,9 +501,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -451,10 +513,12 @@
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="1"/>
     <col min="5" max="5" width="12.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -465,13 +529,22 @@
         <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -487,8 +560,17 @@
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -504,8 +586,17 @@
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
@@ -518,120 +609,217 @@
       <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
+      <c r="F9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="F11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="1" t="s">
+      <c r="F12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" s="1" t="s">
+      <c r="F14" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="F15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>